<commit_message>
Tests zum Upload durchgeführt
</commit_message>
<xml_diff>
--- a/Testing/Use Case based Testing.xlsx
+++ b/Testing/Use Case based Testing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\GitHub\SoftwareHeros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\GitHub\SoftwareHeros\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0EEE55-0E17-4C3E-A7CC-057E858CBF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B96360-4B41-4AC6-BC39-7FA3D9460606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8F0B6F25-0A00-6E48-9C26-F9E73014E07C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Test Design - Use Case based" sheetId="1" r:id="rId1"/>
     <sheet name="Test Reports" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -78,9 +81,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Branch, Version</t>
-  </si>
-  <si>
     <t>Alternative Flow 1</t>
   </si>
   <si>
@@ -175,6 +175,96 @@
   </si>
   <si>
     <t>Admin bei erster Abfrage, Meldung mit ok bestätigen, admin bei zweiter Abfrage, Meldung mit ok bestätigen</t>
+  </si>
+  <si>
+    <t>2, Upload</t>
+  </si>
+  <si>
+    <t>Test database()</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einen unterstützten Pfad an, bestätige TypeCheckMeldung, Dateinamen angeben, yes eingeben</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einen nicht unterstützten Pfad an, TypeCheckMeldung mit ok bestätigen</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: Dokumententyp nicht unterstützt, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>nicht unterstützter Dokumententyp</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einen unterstützten Pfad an, bestätige TypeCheckMeldung, Dateinamen angeben den es schon gibt, yes eingeben</t>
+  </si>
+  <si>
+    <t>Erfolgsmeldung in der Konsole, Überschriten der existierenden Datei, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Dokumentenname existiert bereits</t>
+  </si>
+  <si>
+    <t>Test database(Dokumentenname schon vorhanden)</t>
+  </si>
+  <si>
+    <t>Upload nicht bestätigen</t>
+  </si>
+  <si>
+    <t>Alternative Flow 4</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einen nicht vorhandenen Pfad an, bestätige TypeCheckMeldung</t>
+  </si>
+  <si>
+    <t>Dokumentenpfad nicht vorhanden</t>
+  </si>
+  <si>
+    <t>Alternative Flow 5</t>
+  </si>
+  <si>
+    <t>Benutzer einen unterstützen Pfad an, bestätige TypeCheckMeldung, keinen Namen eingeben, yes eingeben</t>
+  </si>
+  <si>
+    <t>Keinen Dokumentennamen angeben</t>
+  </si>
+  <si>
+    <t>Alternative Flow 6</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: file save failed, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Erfolgsmeldung mit dem Pfad, Speichern der Datei, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Aslanmirza</t>
+  </si>
+  <si>
+    <t>Benutzer gibt Pfadendung an, bestätige TypeCheckMeldung, existierenden Namen eingeben, yes eingeben</t>
+  </si>
+  <si>
+    <t>nur Pfadendung und vorhandener Name</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einen unterstützten Pfad an, bestätige TypeCheckMeldung, Dateinamen angeben, no eingeben, yes</t>
+  </si>
+  <si>
+    <t>Meldung: File not saved, Datei nicht speichern, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Datei gespeichert auf auf null gesetzt</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: Datei nicht gespeichert, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Alte Datei löschen ohne neue zu Speichern</t>
+  </si>
+  <si>
+    <t>Branch</t>
   </si>
 </sst>
 </file>
@@ -565,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EFA617-FEF3-1540-8735-957D00343B99}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -576,7 +666,7 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="92.375" customWidth="1"/>
+    <col min="4" max="4" width="123.5" customWidth="1"/>
     <col min="5" max="5" width="22.875" style="3" customWidth="1"/>
     <col min="6" max="6" width="34.375" style="3" customWidth="1"/>
     <col min="7" max="7" width="32.625" customWidth="1"/>
@@ -610,19 +700,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -630,22 +720,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -653,22 +743,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,22 +766,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -699,19 +789,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -719,22 +809,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -742,22 +832,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -765,97 +855,180 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -866,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E44AE7-7B0E-454D-A297-BCD6EF9884C1}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -878,7 +1051,8 @@
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="15.375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="7" width="15.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="7" max="7" width="26.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -889,7 +1063,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -912,13 +1086,13 @@
         <v>0.49444444444444446</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -935,13 +1109,13 @@
         <v>0.49513888888888885</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -958,13 +1132,13 @@
         <v>0.49652777777777773</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -981,13 +1155,13 @@
         <v>0.49722222222222223</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1004,13 +1178,13 @@
         <v>0.49791666666666662</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1027,13 +1201,13 @@
         <v>0.49861111111111112</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1050,13 +1224,13 @@
         <v>0.49861111111111112</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1073,13 +1247,13 @@
         <v>0.5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1088,8 +1262,163 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.89166666666666661</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.89236111111111116</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.89722222222222225</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.90555555555555556</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.90625</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.90694444444444444</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576 G4 G9">
+  <conditionalFormatting sqref="F1:F1048576 G4 G9 G12 G16">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Suche nach Dokumenten programmiert
#7 Search programmiert und getestet
</commit_message>
<xml_diff>
--- a/Testing/Use Case based Testing.xlsx
+++ b/Testing/Use Case based Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\GitHub\SoftwareHeros\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B96360-4B41-4AC6-BC39-7FA3D9460606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBF3AD-C5A6-45F4-944B-2415D3AFD2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8F0B6F25-0A00-6E48-9C26-F9E73014E07C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{8F0B6F25-0A00-6E48-9C26-F9E73014E07C}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Design - Use Case based" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -265,6 +265,63 @@
   </si>
   <si>
     <t>Branch</t>
+  </si>
+  <si>
+    <t>7, Search</t>
+  </si>
+  <si>
+    <t>Benutzerinput pdf und mit OK bestätigen</t>
+  </si>
+  <si>
+    <t>Test database(Dokumente .pdf, cdew.pdf und test2009.pdf vorhanden)</t>
+  </si>
+  <si>
+    <t>Meldung mit Liste der drei Dokumente .pdf, cdew.pdf und test2009.pdf</t>
+  </si>
+  <si>
+    <t>Bei Abfrage auf Input abbrechen wählen</t>
+  </si>
+  <si>
+    <t>Benutzerinput PDF und mit OK bestätigen</t>
+  </si>
+  <si>
+    <t>Test database(Ohne Dokumente mit PDF im Namen)</t>
+  </si>
+  <si>
+    <t>Da keine Dokumente gefunden wurden soll der Benutzer erneut Input geben</t>
+  </si>
+  <si>
+    <t>Test für Extension 3a nach Cockburn Template</t>
+  </si>
+  <si>
+    <t>Der Benutzer erhält eine leere Meldung und landet wieder im Menü anstatt direkt neuen Input geben zu können</t>
+  </si>
+  <si>
+    <t>Test für Extension 3b nach Cockburn Template</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll nach einem Fehler beim Suchen wieder Input geben können, aber ich kann keinen Fehler erzwingen</t>
+  </si>
+  <si>
+    <t>Benutzerinput ist leer und mit OK bestätigen</t>
+  </si>
+  <si>
+    <t>Test database(Dokumente vorhanden)</t>
+  </si>
+  <si>
+    <t>Alle vorhandenen Dokumente werden angezeigt</t>
+  </si>
+  <si>
+    <t>Benutzerinput ist identisch mit einem Dokumentenamen</t>
+  </si>
+  <si>
+    <t>Benutzerinput cdew.pdf und mit OK bestätigen</t>
+  </si>
+  <si>
+    <t>Test database(cdew.pdf vorhanden)</t>
+  </si>
+  <si>
+    <t>Meldung enthält nur das Dokument cdew.pdf</t>
   </si>
 </sst>
 </file>
@@ -655,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EFA617-FEF3-1540-8735-957D00343B99}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1088,126 @@
         <v>68</v>
       </c>
     </row>
+    <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1039,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E44AE7-7B0E-454D-A297-BCD6EF9884C1}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1417,8 +1594,134 @@
         <v>74</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.69166666666666676</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.69305555555555554</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.69513888888888886</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>45132</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.6972222222222223</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576 G4 G9 G12 G16">
+  <conditionalFormatting sqref="F1:F1048576 G4 G9 G12 G16 G19:G20">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>

</xml_diff>